<commit_message>
Update email template and refresh token in configuration files
</commit_message>
<xml_diff>
--- a/job list.xlsx
+++ b/job list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\offic\OneDrive\Desktop\test\gmail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412E26B4-B374-4955-A08B-D15BDAB1B16A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC3EA9E-B7CA-481D-93FA-0255B04BE354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="268">
   <si>
     <t>Precision AQ</t>
   </si>
@@ -823,6 +823,12 @@
   </si>
   <si>
     <t>https://www.linkedin.com/jobs/view/4253930279/?refId=9JKaC9nZSRqPOd8sWu0WLA%3D%3D&amp;trackingId=JXO7S1X5RlGw1Ij%2FdXar0w%3D%3D</t>
+  </si>
+  <si>
+    <t>referred</t>
+  </si>
+  <si>
+    <t>rejected</t>
   </si>
 </sst>
 </file>
@@ -1216,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E78" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2357,6 +2363,9 @@
       <c r="C90" s="10" t="s">
         <v>216</v>
       </c>
+      <c r="E90" t="s">
+        <v>88</v>
+      </c>
       <c r="F90" t="s">
         <v>217</v>
       </c>
@@ -2371,6 +2380,9 @@
       <c r="D91" t="s">
         <v>221</v>
       </c>
+      <c r="E91" t="s">
+        <v>266</v>
+      </c>
       <c r="F91" t="s">
         <v>220</v>
       </c>
@@ -2395,6 +2407,9 @@
       </c>
       <c r="D93" t="s">
         <v>232</v>
+      </c>
+      <c r="E93" t="s">
+        <v>267</v>
       </c>
       <c r="F93" t="s">
         <v>227</v>

</xml_diff>